<commit_message>
Added single ion salt experiments KCl MgCl2 to master table, rerunning SCM to match updated data, calculate data for CaCl2
</commit_message>
<xml_diff>
--- a/Sorption Experiments/ExperimentDataTemplate _NoScript.xlsx
+++ b/Sorption Experiments/ExperimentDataTemplate _NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="131">
   <si>
     <t>Parameters</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>cps-&gt;Bq (background, Stds, and RaStock 5)</t>
+  </si>
+  <si>
+    <t>MinMass (g)</t>
+  </si>
+  <si>
+    <t>sMinMass (g)</t>
+  </si>
+  <si>
+    <t>Ncount</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -789,11 +797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227970112"/>
-        <c:axId val="235474464"/>
+        <c:axId val="189401656"/>
+        <c:axId val="189402048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227970112"/>
+        <c:axId val="189401656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,19 +823,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235474464"/>
+        <c:crossAx val="189402048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235474464"/>
+        <c:axId val="189402048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,21 +856,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227970112"/>
+        <c:crossAx val="189401656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -908,7 +913,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1093,11 +1097,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235468584"/>
-        <c:axId val="235468976"/>
+        <c:axId val="193315384"/>
+        <c:axId val="193317736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235468584"/>
+        <c:axId val="193315384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,19 +1123,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235468976"/>
+        <c:crossAx val="193317736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235468976"/>
+        <c:axId val="193317736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,21 +1156,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235468584"/>
+        <c:crossAx val="193315384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1283,140 +1284,6 @@
         <row r="2">
           <cell r="D2">
             <v>1.1544444444444444</v>
-          </cell>
-          <cell r="G2">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3">
-            <v>3.5588888888888888</v>
-          </cell>
-          <cell r="G3">
-            <v>0.42769009531437396</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>14.189444444444446</v>
-          </cell>
-          <cell r="G4">
-            <v>2.1384504765718702</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>27.261666666666667</v>
-          </cell>
-          <cell r="G5">
-            <v>4.2769009531437403</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>133.3138888888889</v>
-          </cell>
-          <cell r="G6">
-            <v>21.384504765718699</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>267.61888888888888</v>
-          </cell>
-          <cell r="G7">
-            <v>42.769009531437398</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>1343.9216666666666</v>
-          </cell>
-          <cell r="G8">
-            <v>213.845047657187</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>5624.5516666666663</v>
-          </cell>
-          <cell r="G9">
-            <v>921.74647887323954</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>0.1441714628506657</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>0.52694379154793525</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>2.2192609148432805</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>4.3002759088928997</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>21.183118079488228</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>42.563623553202696</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>213.90420976854736</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="B72">
-            <v>-0.86244335302746633</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="B73">
-            <v>-0.46848823374427229</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="B74">
-            <v>1.273270363178999</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="B75">
-            <v>3.4150827376553288</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="B76">
-            <v>20.791161420752843</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="B77">
-            <v>42.796303780178178</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="B78">
-            <v>219.142648643325</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="B79">
-            <v>920.50054699429393</v>
           </cell>
         </row>
       </sheetData>
@@ -1697,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -7067,15 +6934,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -7106,8 +6973,20 @@
       <c r="J1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7144,7 +7023,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -7185,7 +7064,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -7226,7 +7105,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -7267,7 +7146,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>250</v>
       </c>
@@ -7308,7 +7187,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>

</xml_diff>